<commit_message>
* Started implementing OOP concepts to decrease script writing time and effort * Added core elements that will be used on all scripts * Divided the locators file into multiple files categorized by the page where these locators operate * Created 3 scenarios that use the new design
</commit_message>
<xml_diff>
--- a/Documents/NopCommerce_Bugs_Report.xlsx
+++ b/Documents/NopCommerce_Bugs_Report.xlsx
@@ -68,9 +68,6 @@
     <t>URL</t>
   </si>
   <si>
-    <t>nopCommerce demo store</t>
-  </si>
-  <si>
     <t>Screenshot</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>The home page promotiona banner only refreshes the home page when clicked</t>
+  </si>
+  <si>
+    <t>https://demo.nopcommerce.com/</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +691,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -700,119 +700,119 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="C9" s="13"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="C12" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>